<commit_message>
Se termina de digitalizar M51, Se implementa compartimientos
</commit_message>
<xml_diff>
--- a/modelo para tomar nota.xlsx
+++ b/modelo para tomar nota.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFBC0DC3-386B-458F-AA27-D853CE0A7A04}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9BF90110-8BAE-4141-AEA7-DC70F211454F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <definedName name="ca">Table4[Categorias]</definedName>
     <definedName name="Categorias">Table4[Categorias]</definedName>
     <definedName name="Medidas">Table5[Medidas]</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Table1[#All]</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Movil 51'!$A$1:$F$18</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -301,9 +301,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -322,6 +319,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -333,24 +333,6 @@
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
         <right/>
         <top style="thin">
           <color indexed="64"/>
@@ -483,6 +465,22 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="thin">
           <color indexed="64"/>
@@ -497,12 +495,14 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
   </dxfs>
@@ -519,15 +519,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F21" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F21" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="A1:F21" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Categoria" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descripcion" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Medidas" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="marca" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="N/ de serie" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cajonera" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Categoria" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descripcion" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Medidas" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="marca" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="N/ de serie" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cajonera" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -837,7 +837,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F21"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,40 +854,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="11"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11"/>
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="10"/>
       <c r="I3" t="s">
         <v>21</v>
       </c>
@@ -897,20 +897,20 @@
       <c r="K3" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10"/>
       <c r="I4" t="s">
         <v>22</v>
       </c>
@@ -925,12 +925,12 @@
       </c>
     </row>
     <row r="5" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="10"/>
       <c r="I5" t="s">
         <v>24</v>
       </c>
@@ -945,12 +945,12 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
       <c r="I6" t="s">
         <v>25</v>
       </c>
@@ -965,12 +965,12 @@
       </c>
     </row>
     <row r="7" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="11"/>
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="10"/>
       <c r="I7" t="s">
         <v>26</v>
       </c>
@@ -985,12 +985,12 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="10"/>
       <c r="I8" t="s">
         <v>27</v>
       </c>
@@ -1005,12 +1005,12 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="11"/>
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="10"/>
       <c r="I9" t="s">
         <v>29</v>
       </c>
@@ -1025,12 +1025,12 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
       <c r="I10" t="s">
         <v>30</v>
       </c>
@@ -1045,12 +1045,12 @@
       </c>
     </row>
     <row r="11" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11"/>
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10"/>
       <c r="I11" t="s">
         <v>31</v>
       </c>
@@ -1062,12 +1062,12 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="10"/>
       <c r="I12" t="s">
         <v>28</v>
       </c>
@@ -1079,12 +1079,12 @@
       </c>
     </row>
     <row r="13" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="11"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="10"/>
       <c r="I13" t="s">
         <v>32</v>
       </c>
@@ -1096,68 +1096,68 @@
       </c>
     </row>
     <row r="14" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="11"/>
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="10"/>
     </row>
     <row r="16" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="10"/>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="11"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="10"/>
     </row>
     <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="10"/>
     </row>
     <row r="19" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="11"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="10"/>
     </row>
     <row r="20" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="10"/>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>